<commit_message>
Initial commit - TechCare project with new UI
</commit_message>
<xml_diff>
--- a/Excel-To-Do-List-.xlsx
+++ b/Excel-To-Do-List-.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Warushi\Desktop\project_official\Tech-Care_official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDCA87C-DAD4-4125-93AE-5C8F520BFFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647C7E79-118C-4D7B-8FDE-2B655C454DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To Do List Check Box" sheetId="6" r:id="rId1"/>
@@ -739,7 +739,7 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.14130434782608695</c:v>
+                  <c:v>0.17391304347826086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,7 +1487,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$E$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1620,7 +1620,7 @@
               <a:cs typeface="Verdana"/>
             </a:rPr>
             <a:pPr algn="ctr"/>
-            <a:t>14.1%</a:t>
+            <a:t>17.4%</a:t>
           </a:fld>
           <a:endParaRPr lang="en-GB" sz="800" b="1" i="1">
             <a:solidFill>
@@ -3659,7 +3659,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -3785,7 +3785,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>7</v>
@@ -3859,7 +3859,7 @@
       </c>
       <c r="H10" s="1">
         <f>COUNTIFS($D$5:$D$29,$H$5,$E$5:$E$29,TRUE)*$I$5+COUNTIFS($D$5:$D$29,$H$6,$E$5:$E$29,TRUE)*$I$6+COUNTIFS($D$5:$D$29,$H$7,$E$5:$E$29,TRUE)*$I$7</f>
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1">
@@ -3907,7 +3907,7 @@
       </c>
       <c r="H12" s="13">
         <f>IFERROR(H10/H11,0)</f>
-        <v>0.14130434782608695</v>
+        <v>0.17391304347826086</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1">

</xml_diff>